<commit_message>
Lassa fever SI calcs
</commit_message>
<xml_diff>
--- a/Clustering/cluster_dat.xlsx
+++ b/Clustering/cluster_dat.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lshjw6/Documents/blueprint/epi_review/clustering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lshjw6/Documents/archetypes/Clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290CE48D-5BD4-EE42-BF8C-81BB05166584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F91833-50E4-B44B-9B20-D59673E60519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{B3940D55-DFC4-2242-BE28-18A04C8C9078}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B3940D55-DFC4-2242-BE28-18A04C8C9078}"/>
   </bookViews>
   <sheets>
-    <sheet name="k-proto" sheetId="8" r:id="rId1"/>
-    <sheet name="route_SI" sheetId="7" r:id="rId2"/>
-    <sheet name="route" sheetId="6" r:id="rId3"/>
-    <sheet name="inc" sheetId="5" r:id="rId4"/>
-    <sheet name="R0_CFR_SI" sheetId="4" r:id="rId5"/>
-    <sheet name="R0_CFR" sheetId="3" r:id="rId6"/>
-    <sheet name="num" sheetId="1" r:id="rId7"/>
-    <sheet name="source doc" sheetId="2" r:id="rId8"/>
+    <sheet name="k-proto_ps" sheetId="10" r:id="rId1"/>
+    <sheet name="k-proto" sheetId="8" r:id="rId2"/>
+    <sheet name="presym" sheetId="9" r:id="rId3"/>
+    <sheet name="route_SI" sheetId="7" r:id="rId4"/>
+    <sheet name="route" sheetId="6" r:id="rId5"/>
+    <sheet name="inc" sheetId="5" r:id="rId6"/>
+    <sheet name="R0_CFR_SI" sheetId="4" r:id="rId7"/>
+    <sheet name="R0_CFR" sheetId="3" r:id="rId8"/>
+    <sheet name="num" sheetId="1" r:id="rId9"/>
+    <sheet name="source doc" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="131">
   <si>
     <t>Pathogen</t>
   </si>
@@ -433,6 +435,9 @@
   </si>
   <si>
     <t xml:space="preserve">animal </t>
+  </si>
+  <si>
+    <t>pre_sym</t>
   </si>
 </sst>
 </file>
@@ -560,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -582,80 +587,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF76A5AF"/>
-          <bgColor rgb="FF76A5AF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6FA8DC"/>
-          <bgColor rgb="FF6FA8DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC27BA0"/>
-          <bgColor rgb="FFC27BA0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF6B26B"/>
-          <bgColor rgb="FFF6B26B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE06666"/>
-          <bgColor rgb="FFE06666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -984,11 +921,1147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB32C75-18A2-6940-BDA7-584583F4D4D3}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.69</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4.82</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.67</v>
+      </c>
+      <c r="E2" s="1">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.47</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="E3" s="1">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.08</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.59</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3.21</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="C6" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>61.1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D7" s="1">
+        <v>61.9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>33.1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>58</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="C9" s="1">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3.02</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D11" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E11" s="8">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3.26</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3.48</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.46</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3.08</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0.18</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>53.5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8.32</v>
+      </c>
+      <c r="D17" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="C18" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5983E3CC-3D3A-3945-B1A0-00FDCBC28BBB}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+    <col min="3" max="7" width="22.83203125" customWidth="1"/>
+    <col min="8" max="8" width="33.83203125" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K9" r:id="rId1" xr:uid="{09601DE1-61A1-0143-93AE-FB2E55B5C3BD}"/>
+    <hyperlink ref="K11" r:id="rId2" xr:uid="{EFF173AB-2D1D-B747-85BD-23E6CA8138D2}"/>
+    <hyperlink ref="K12" r:id="rId3" xr:uid="{D2E678BD-6146-B64F-B361-6CE18E594623}"/>
+    <hyperlink ref="K13" r:id="rId4" location=":~:text=Mpox%20can%20be%20transmitted%20through,newborn%20during%20or%20after%20birth." xr:uid="{7DAF30C5-45E8-6948-BF18-5E4CE1EDF5F7}"/>
+    <hyperlink ref="K14" r:id="rId5" xr:uid="{2172DAEF-F0AF-0249-9D09-6B5252E7CC4A}"/>
+    <hyperlink ref="K15" r:id="rId6" xr:uid="{2EC38D6E-C57F-CD49-9270-9D818E969B94}"/>
+    <hyperlink ref="K16" r:id="rId7" xr:uid="{C95DFB2F-9000-2B4D-B556-1EA008F91B53}"/>
+    <hyperlink ref="K17" r:id="rId8" xr:uid="{27BF3130-3BD5-674D-974C-293920934DB4}"/>
+    <hyperlink ref="K18" r:id="rId9" location="sec5" xr:uid="{769D7377-F493-3F43-87FC-2B5DD0D91B2F}"/>
+    <hyperlink ref="K19" r:id="rId10" location="Sec3" xr:uid="{4B202C53-E78A-3647-916E-1C6142D24A21}"/>
+    <hyperlink ref="K20" r:id="rId11" location="Sec3" display="https://www.nature.com/articles/nrmicro.2016.81#Sec3" xr:uid="{0967C889-87E1-F949-9CBC-C12727634FA6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2244612A-0C82-FB4B-A832-5505F6652CB8}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,13 +2102,13 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="1">
         <v>2.69</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="1">
         <v>4.82</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="1">
         <v>2.67</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1052,13 +2125,13 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="1">
         <v>4.4800000000000004</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="1">
         <v>3.47</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="1">
         <v>2.62</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1075,13 +2148,13 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="1">
         <v>5.08</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="1">
         <v>3.59</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="1">
         <v>2.0099999999999998</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1098,13 +2171,13 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="1">
         <v>9.5</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="1">
         <v>3.21</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="1">
         <v>0.7</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1121,13 +2194,13 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="1">
         <v>1.95</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="1">
         <v>15.4</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="1">
         <v>61.1</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1144,13 +2217,13 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="1">
         <v>0.8</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="1">
         <v>61.9</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1167,13 +2240,13 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="1">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="1">
         <v>7.8</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="1">
         <v>33.1</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1190,13 +2263,13 @@
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="1">
         <v>0.33</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="1">
         <v>13</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="1">
         <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1213,13 +2286,13 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="1">
         <v>3.02</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="1">
         <v>12</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="8">
         <v>0.02</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1236,13 +2309,13 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="1">
         <v>1.8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="1">
         <v>8.5</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="8">
         <v>8.6999999999999993</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1259,13 +2332,13 @@
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="1">
         <v>1.8</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="1">
         <v>3.26</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="1">
         <v>2.5</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1282,13 +2355,13 @@
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="1">
         <v>1.65</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="1">
         <v>3.5</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="1">
         <v>0.2</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1305,13 +2378,13 @@
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="1">
         <v>1.8</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="1">
         <v>3.48</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="1">
         <v>0.2</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1328,13 +2401,13 @@
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="1">
         <v>1.46</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="1">
         <v>3.08</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="1">
         <v>0.02</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1351,13 +2424,13 @@
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="18">
         <v>0.18</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="1">
         <v>6.8</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="1">
         <v>53.5</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1374,13 +2447,13 @@
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="1">
         <v>2.9</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="1">
         <v>8.32</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="1">
         <v>9.6</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1397,13 +2470,13 @@
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="1">
         <v>0.95</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="1">
         <v>12.6</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="1">
         <v>39.1</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -1421,12 +2494,603 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A25BF62-03BE-F349-AC94-E2DE1E389ACC}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.69</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4.82</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.67</v>
+      </c>
+      <c r="E2" s="1">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.47</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="E3" s="1">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.08</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.59</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3.21</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="C6" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>61.1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D7" s="1">
+        <v>61.9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>33.1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>58</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="C9" s="1">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3.02</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="D11" s="8">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E11" s="8">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3.26</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3.48</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.46</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3.08</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="18">
+        <v>0.18</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="D16" s="1">
+        <v>53.5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8.32</v>
+      </c>
+      <c r="D17" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="C18" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F74BD6-5FB4-0248-BB9E-3B98CE49ECAB}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection sqref="A1:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1470,13 +3134,13 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="1">
         <v>2.69</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="1">
         <v>4.82</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="1">
         <v>2.67</v>
       </c>
       <c r="E2" s="1">
@@ -1499,13 +3163,13 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="1">
         <v>4.4800000000000004</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="1">
         <v>3.47</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="1">
         <v>2.62</v>
       </c>
       <c r="E3" s="1">
@@ -1528,13 +3192,13 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="1">
         <v>5.08</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="1">
         <v>3.59</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="1">
         <v>2.0099999999999998</v>
       </c>
       <c r="E4" s="1">
@@ -1557,13 +3221,13 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="1">
         <v>9.5</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="1">
         <v>3.21</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="1">
         <v>0.7</v>
       </c>
       <c r="E5" s="1">
@@ -1586,13 +3250,13 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="1">
         <v>1.95</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="1">
         <v>15.4</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="1">
         <v>61.1</v>
       </c>
       <c r="E6" s="1">
@@ -1615,13 +3279,13 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="1">
         <v>0.8</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="1">
         <v>61.9</v>
       </c>
       <c r="E7" s="1">
@@ -1644,13 +3308,13 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="1">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="1">
         <v>7.8</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="1">
         <v>33.1</v>
       </c>
       <c r="E8" s="1">
@@ -1673,13 +3337,13 @@
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="1">
         <v>0.33</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="1">
         <v>13</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="1">
         <v>61</v>
       </c>
       <c r="E9" s="1">
@@ -1702,13 +3366,13 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="1">
         <v>3.02</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="1">
         <v>12</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="8">
         <v>0.02</v>
       </c>
       <c r="E10" s="1">
@@ -1731,13 +3395,13 @@
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="1">
         <v>1.8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="1">
         <v>8.5</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="8">
         <v>8.6999999999999993</v>
       </c>
       <c r="E11" s="1">
@@ -1760,13 +3424,13 @@
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="1">
         <v>1.8</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="1">
         <v>3.26</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="1">
         <v>2.5</v>
       </c>
       <c r="E12" s="1">
@@ -1789,13 +3453,13 @@
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="1">
         <v>1.65</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="1">
         <v>3.5</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="1">
         <v>0.2</v>
       </c>
       <c r="E13" s="1">
@@ -1818,13 +3482,13 @@
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="1">
         <v>1.8</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="1">
         <v>3.48</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="1">
         <v>0.2</v>
       </c>
       <c r="E14" s="1">
@@ -1847,13 +3511,13 @@
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="1">
         <v>1.46</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="1">
         <v>3.08</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="1">
         <v>0.02</v>
       </c>
       <c r="E15" s="1">
@@ -1876,13 +3540,13 @@
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="18">
         <v>0.18</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="1">
         <v>6.8</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="1">
         <v>53.5</v>
       </c>
       <c r="E16" s="1">
@@ -1905,13 +3569,13 @@
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="1">
         <v>2.9</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="1">
         <v>8.32</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="1">
         <v>9.6</v>
       </c>
       <c r="E17" s="1">
@@ -1934,13 +3598,13 @@
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="1">
         <v>0.95</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="1">
         <v>12.6</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="1">
         <v>39.1</v>
       </c>
       <c r="E18" s="1">
@@ -1964,7 +3628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292CB424-D5BB-DB45-813C-F60D6631A284}">
   <dimension ref="A1:H20"/>
   <sheetViews>
@@ -2505,7 +4169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00E9493-6F8F-D540-A467-D7EC86C53227}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -2826,7 +4490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C9DDD5-EBAE-934B-8DA8-DADE9DB93842}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -3096,7 +4760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4826DE6F-38CE-124E-809F-C969EAD33B3A}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -3334,7 +4998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9EAC15-683C-1044-B046-5E5CE56F9DFA}">
   <dimension ref="A1:I20"/>
   <sheetViews>
@@ -3855,657 +5519,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5983E3CC-3D3A-3945-B1A0-00FDCBC28BBB}">
-  <dimension ref="A1:K20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K19" sqref="K19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="35.5" customWidth="1"/>
-    <col min="3" max="7" width="22.83203125" customWidth="1"/>
-    <col min="8" max="8" width="33.83203125" customWidth="1"/>
-    <col min="9" max="9" width="22.83203125" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="K17" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K18" s="16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K9" r:id="rId1" xr:uid="{09601DE1-61A1-0143-93AE-FB2E55B5C3BD}"/>
-    <hyperlink ref="K11" r:id="rId2" xr:uid="{EFF173AB-2D1D-B747-85BD-23E6CA8138D2}"/>
-    <hyperlink ref="K12" r:id="rId3" xr:uid="{D2E678BD-6146-B64F-B361-6CE18E594623}"/>
-    <hyperlink ref="K13" r:id="rId4" location=":~:text=Mpox%20can%20be%20transmitted%20through,newborn%20during%20or%20after%20birth." xr:uid="{7DAF30C5-45E8-6948-BF18-5E4CE1EDF5F7}"/>
-    <hyperlink ref="K14" r:id="rId5" xr:uid="{2172DAEF-F0AF-0249-9D09-6B5252E7CC4A}"/>
-    <hyperlink ref="K15" r:id="rId6" xr:uid="{2EC38D6E-C57F-CD49-9270-9D818E969B94}"/>
-    <hyperlink ref="K16" r:id="rId7" xr:uid="{C95DFB2F-9000-2B4D-B556-1EA008F91B53}"/>
-    <hyperlink ref="K17" r:id="rId8" xr:uid="{27BF3130-3BD5-674D-974C-293920934DB4}"/>
-    <hyperlink ref="K18" r:id="rId9" location="sec5" xr:uid="{769D7377-F493-3F43-87FC-2B5DD0D91B2F}"/>
-    <hyperlink ref="K19" r:id="rId10" location="Sec3" xr:uid="{4B202C53-E78A-3647-916E-1C6142D24A21}"/>
-    <hyperlink ref="K20" r:id="rId11" location="Sec3" display="https://www.nature.com/articles/nrmicro.2016.81#Sec3" xr:uid="{0967C889-87E1-F949-9CBC-C12727634FA6}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>